<commit_message>
Expand "Template Document" field
Now includes the full name of each template document rather than just the partial name.
</commit_message>
<xml_diff>
--- a/src/resources/templates/excel/text_block_templates.xlsx
+++ b/src/resources/templates/excel/text_block_templates.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason D'Amico\Documents\cdf\pgov-cover-sheet-reader\src\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason D'Amico\Documents\cdf\pgov-cover-sheet-reader\src\resources\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23131A28-33F8-4D44-AA68-55C3790B6D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72673739-1391-4001-B270-3D366479FCCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,15 +22,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
-    <t>Template Document</t>
-  </si>
-  <si>
     <t>Context</t>
   </si>
   <si>
-    <t>Summary_Report</t>
-  </si>
-  <si>
     <t>Sentence Template Neutral</t>
   </si>
   <si>
@@ -46,9 +40,6 @@
     <t>speedometer_text</t>
   </si>
   <si>
-    <t>APG_Summary</t>
-  </si>
-  <si>
     <t>Underneath speedometer (current status) graphic on each APG page.</t>
   </si>
   <si>
@@ -89,6 +80,15 @@
   </si>
   <si>
     <t>**{challenge}** has been reported as challenge for the **{goal}** team in each of the last **{challenge count} quarters**.</t>
+  </si>
+  <si>
+    <t>Summary_Report_Template</t>
+  </si>
+  <si>
+    <t>APG_Summary_Template</t>
+  </si>
+  <si>
+    <t>Template Document Name</t>
   </si>
 </sst>
 </file>
@@ -958,9 +958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -975,82 +973,82 @@
   <sheetData>
     <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Include mention that `recurring_challenge_text` is in its template document
</commit_message>
<xml_diff>
--- a/src/resources/templates/excel/text_block_templates.xlsx
+++ b/src/resources/templates/excel/text_block_templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason D'Amico\Documents\cdf\pgov-cover-sheet-reader\src\resources\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72673739-1391-4001-B270-3D366479FCCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5A3CA2-D1B9-4F6D-A7D9-1FDA7D40C117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Context</t>
   </si>
@@ -958,7 +958,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1033,6 +1035,9 @@
       <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">

</xml_diff>

<commit_message>
Add reference to README in text block templates document
Required updating the pandas retrieval of the file to skip the first row.
</commit_message>
<xml_diff>
--- a/src/resources/templates/excel/text_block_templates.xlsx
+++ b/src/resources/templates/excel/text_block_templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason D'Amico\Documents\cdf\pgov-cover-sheet-reader\src\resources\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5A3CA2-D1B9-4F6D-A7D9-1FDA7D40C117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FC6FA4-5737-497E-8F92-ED984C2AE353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Context</t>
   </si>
@@ -89,13 +89,37 @@
   </si>
   <si>
     <t>Template Document Name</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>README</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+This document stores all of the text templates that will be dynamically inserted into the template documents. For more guidance on how to edit this document and change the sentences dynamically inserted into the summary report, please read this project's README.md file, which may be found locally or on the home page of this repository on GitHub.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +254,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -418,7 +458,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -548,8 +588,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -592,8 +641,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -601,8 +651,14 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -636,6 +692,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -956,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -973,90 +1030,103 @@
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="144" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="144" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="5" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Correct typo in `recurring_challenge_text` template
</commit_message>
<xml_diff>
--- a/src/resources/templates/excel/text_block_templates.xlsx
+++ b/src/resources/templates/excel/text_block_templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason D'Amico\Documents\cdf\pgov-cover-sheet-reader\src\resources\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FC6FA4-5737-497E-8F92-ED984C2AE353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C542F368-B671-47DB-824C-A64A4288FB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>recurring_challenge_text</t>
-  </si>
-  <si>
-    <t>**{challenge}** has been reported as challenge for the **{goal}** team in each of the last **{challenge count} quarters**.</t>
   </si>
   <si>
     <t>Summary_Report_Template</t>
@@ -113,6 +110,9 @@
       <t xml:space="preserve">
 This document stores all of the text templates that will be dynamically inserted into the template documents. For more guidance on how to edit this document and change the sentences dynamically inserted into the summary report, please read this project's README.md file, which may be found locally or on the home page of this repository on GitHub.</t>
     </r>
+  </si>
+  <si>
+    <t>**{challenge}** has been reported as a challenge for the **{goal}** team in each of the last **{challenge count} quarters**.</t>
   </si>
 </sst>
 </file>
@@ -651,11 +651,11 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1015,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1031,18 +1031,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
+      <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>14</v>
@@ -1068,7 +1068,7 @@
     </row>
     <row r="3" spans="1:8" ht="144" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
@@ -1091,7 +1091,7 @@
     </row>
     <row r="4" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>18</v>
@@ -1100,7 +1100,7 @@
         <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>16</v>
@@ -1108,7 +1108,7 @@
     </row>
     <row r="5" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>

</xml_diff>